<commit_message>
cleaned up Excel file; still involves a lot of manual tweaking
</commit_message>
<xml_diff>
--- a/forest-plot/metadata.xlsx
+++ b/forest-plot/metadata.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agrogan\Box Sync\Box Sync\GitHub\teaching\forest-plot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agrogan/Box Sync/GitHub/teaching/forest-plot/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83D9E00-0427-9E47-BF05-A971DD1CC692}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -57,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -611,7 +623,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -664,7 +675,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1490,7 +1501,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1770,19 +1787,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1808,7 +1825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1839,7 +1856,7 @@
         <v>0.10000000000000009</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1870,7 +1887,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>